<commit_message>
Final with Crosswalk Contribution Form
</commit_message>
<xml_diff>
--- a/NIST-Privacy-Framework-Version1-Crosswalk-SLC- FIPPs-NIST PF.xlsx
+++ b/NIST-Privacy-Framework-Version1-Crosswalk-SLC- FIPPs-NIST PF.xlsx
@@ -6,6 +6,7 @@
     <sheet state="visible" name="Privacy Framework to Source" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Source to Privacy Framework" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Summary" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Crosswalk Contribution Form" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="208">
   <si>
     <t>NIST Privacy Framework Version 1.0 to FIPPs Crosswalk</t>
   </si>
@@ -2850,12 +2851,51 @@
   <si>
     <t>9.Transparency</t>
   </si>
+  <si>
+    <t>Crosswalk Contribution Form</t>
+  </si>
+  <si>
+    <t>Contributor: Dr. Sarah L. Cortes, Northeastern University</t>
+  </si>
+  <si>
+    <t>Contributor GitHub Username: @SarahCortes</t>
+  </si>
+  <si>
+    <t>Resource: (GitHub directory)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Related Documentation: </t>
+  </si>
+  <si>
+    <t>Crosswalk Name: NIST Privacy Framework 1.0-FIPPs Crosswalk</t>
+  </si>
+  <si>
+    <t>Source Name: FIPPs: Fair Information Privacy Practices (FIPPs)</t>
+  </si>
+  <si>
+    <t>Link to Source: https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/circulars/A130/a130revised.pdf</t>
+  </si>
+  <si>
+    <t>Source Type: Guideline</t>
+  </si>
+  <si>
+    <t>laws and regulations,</t>
+  </si>
+  <si>
+    <t>standard, or</t>
+  </si>
+  <si>
+    <t>framework.</t>
+  </si>
+  <si>
+    <t>Contributor Notes: FIPPs are high-level and older. This uses the 2016 White House OMB version of the FIPPs.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -2981,6 +3021,16 @@
       <sz val="12.0"/>
       <color theme="1"/>
       <name val="&quot;Netflix Sans&quot;"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF24292E"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF24292E"/>
+      <name val="-apple-system"/>
     </font>
   </fonts>
   <fills count="18">
@@ -3341,7 +3391,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="94">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
     </xf>
@@ -3615,6 +3665,15 @@
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="16" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="16" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="16" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -3632,6 +3691,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -34534,4 +34597,114 @@
   </hyperlinks>
   <drawing r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="91" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="92"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="91" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="92"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="91" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="92"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="91" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="92"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="91" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="92"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="91" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="92"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="91" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="92"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="91" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="92"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="91" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="92"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="93" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="93" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="93" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" s="93"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="91" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>